<commit_message>
dont show cpa/tcpa if tcpa is negative (ie we have passed it)
</commit_message>
<xml_diff>
--- a/docs/requests-and-responses.xlsx
+++ b/docs/requests-and-responses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/git/vesper-watchmate-mobile-app-broker/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9B6F52-8EA8-714F-BA66-294540693D1B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91D0C63-B8BF-C74B-82FB-525000EBB00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{4792B55F-C504-B641-BF90-4586F2D067A0}"/>
   </bookViews>
@@ -510,8 +510,8 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>